<commit_message>
changed xlsx to keep sections
</commit_message>
<xml_diff>
--- a/F17_meen_classes.xlsx
+++ b/F17_meen_classes.xlsx
@@ -14,17 +14,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="159">
   <si>
     <t>index</t>
   </si>
   <si>
+    <t>Class #</t>
+  </si>
+  <si>
     <t xml:space="preserve">Subject </t>
   </si>
   <si>
     <t>Cat. #</t>
   </si>
   <si>
+    <t>Sec.</t>
+  </si>
+  <si>
     <t>Component</t>
   </si>
   <si>
@@ -32,6 +38,177 @@
   </si>
   <si>
     <t>Instructor</t>
+  </si>
+  <si>
+    <t>1358</t>
+  </si>
+  <si>
+    <t>1359</t>
+  </si>
+  <si>
+    <t>17295</t>
+  </si>
+  <si>
+    <t>10352</t>
+  </si>
+  <si>
+    <t>11250</t>
+  </si>
+  <si>
+    <t>11251</t>
+  </si>
+  <si>
+    <t>12271</t>
+  </si>
+  <si>
+    <t>17327</t>
+  </si>
+  <si>
+    <t>14934</t>
+  </si>
+  <si>
+    <t>18881</t>
+  </si>
+  <si>
+    <t>17326</t>
+  </si>
+  <si>
+    <t>17328</t>
+  </si>
+  <si>
+    <t>1367</t>
+  </si>
+  <si>
+    <t>13124</t>
+  </si>
+  <si>
+    <t>17314</t>
+  </si>
+  <si>
+    <t>17315</t>
+  </si>
+  <si>
+    <t>17317</t>
+  </si>
+  <si>
+    <t>1371</t>
+  </si>
+  <si>
+    <t>10805</t>
+  </si>
+  <si>
+    <t>2523</t>
+  </si>
+  <si>
+    <t>10807</t>
+  </si>
+  <si>
+    <t>1368</t>
+  </si>
+  <si>
+    <t>17303</t>
+  </si>
+  <si>
+    <t>1369</t>
+  </si>
+  <si>
+    <t>13593</t>
+  </si>
+  <si>
+    <t>12272</t>
+  </si>
+  <si>
+    <t>18870</t>
+  </si>
+  <si>
+    <t>18868</t>
+  </si>
+  <si>
+    <t>7246</t>
+  </si>
+  <si>
+    <t>11397</t>
+  </si>
+  <si>
+    <t>13125</t>
+  </si>
+  <si>
+    <t>16144</t>
+  </si>
+  <si>
+    <t>13751</t>
+  </si>
+  <si>
+    <t>17316</t>
+  </si>
+  <si>
+    <t>17318</t>
+  </si>
+  <si>
+    <t>1940</t>
+  </si>
+  <si>
+    <t>10806</t>
+  </si>
+  <si>
+    <t>2522</t>
+  </si>
+  <si>
+    <t>13932</t>
+  </si>
+  <si>
+    <t>10808</t>
+  </si>
+  <si>
+    <t>1941</t>
+  </si>
+  <si>
+    <t>17304</t>
+  </si>
+  <si>
+    <t>1942</t>
+  </si>
+  <si>
+    <t>18314</t>
+  </si>
+  <si>
+    <t>12273</t>
+  </si>
+  <si>
+    <t>18871</t>
+  </si>
+  <si>
+    <t>18869</t>
+  </si>
+  <si>
+    <t>7247</t>
+  </si>
+  <si>
+    <t>11398</t>
+  </si>
+  <si>
+    <t>13126</t>
+  </si>
+  <si>
+    <t>16145</t>
+  </si>
+  <si>
+    <t>14082</t>
+  </si>
+  <si>
+    <t>17302</t>
+  </si>
+  <si>
+    <t>17301</t>
+  </si>
+  <si>
+    <t>5973</t>
+  </si>
+  <si>
+    <t>11386</t>
+  </si>
+  <si>
+    <t>17319</t>
   </si>
   <si>
     <t>ME EN</t>
@@ -671,13 +848,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,100 +873,118 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2">
         <v>1000</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3">
         <v>1000</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
+      <c r="F3">
+        <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4">
         <v>1000</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F4">
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5">
         <v>1010</v>
       </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
+      <c r="F5">
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -797,22 +992,28 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6">
         <v>2010</v>
       </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
+      <c r="F6">
+        <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -820,45 +1021,54 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7">
         <v>2030</v>
       </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
+      <c r="F7">
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8">
         <v>2450</v>
       </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
+      <c r="F8">
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -866,45 +1076,54 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9">
         <v>2550</v>
       </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
+      <c r="F9">
+        <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10">
         <v>2650</v>
       </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
+      <c r="F10">
+        <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -912,22 +1131,28 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11">
         <v>2960</v>
       </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
+      <c r="F11">
+        <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>67</v>
+      </c>
+      <c r="H11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -935,22 +1160,28 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12">
         <v>2960</v>
       </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" t="s">
-        <v>16</v>
+      <c r="F12">
+        <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>67</v>
+      </c>
+      <c r="H12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -958,22 +1189,28 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13">
         <v>2960</v>
       </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
+      <c r="F13">
+        <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>67</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -981,22 +1218,28 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14">
         <v>3000</v>
       </c>
-      <c r="E14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
+      <c r="F14">
+        <v>1</v>
       </c>
       <c r="G14" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1004,68 +1247,80 @@
         <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15">
         <v>3220</v>
       </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" t="s">
-        <v>18</v>
+      <c r="F15">
+        <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16">
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16">
         <v>3230</v>
       </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" t="s">
-        <v>19</v>
+      <c r="F16">
+        <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17">
         <v>3300</v>
       </c>
-      <c r="E17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" t="s">
-        <v>20</v>
+      <c r="F17">
+        <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H17" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1073,22 +1328,28 @@
         <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18">
         <v>3400</v>
       </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" t="s">
-        <v>21</v>
+      <c r="F18">
+        <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H18" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1096,45 +1357,54 @@
         <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19">
         <v>3400</v>
       </c>
-      <c r="E19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" t="s">
-        <v>21</v>
+      <c r="F19">
+        <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H19" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
         <v>75</v>
       </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20">
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20">
         <v>3600</v>
       </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" t="s">
-        <v>22</v>
+      <c r="F20">
+        <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H20" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1142,68 +1412,80 @@
         <v>82</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21">
         <v>3610</v>
       </c>
-      <c r="E21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" t="s">
-        <v>23</v>
+      <c r="F21">
+        <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
         <v>83</v>
       </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22">
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22">
         <v>3650</v>
       </c>
-      <c r="E22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" t="s">
-        <v>24</v>
+      <c r="F22">
+        <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H22" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
         <v>90</v>
       </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23">
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23">
         <v>3700</v>
       </c>
-      <c r="E23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" t="s">
-        <v>25</v>
+      <c r="F23">
+        <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H23" t="s">
+        <v>84</v>
+      </c>
+      <c r="I23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1211,22 +1493,28 @@
         <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24">
         <v>3710</v>
       </c>
-      <c r="E24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" t="s">
-        <v>25</v>
+      <c r="F24">
+        <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H24" t="s">
+        <v>84</v>
+      </c>
+      <c r="I24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1234,22 +1522,28 @@
         <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25">
         <v>4000</v>
       </c>
-      <c r="E25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" t="s">
-        <v>26</v>
+      <c r="F25">
+        <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H25" t="s">
+        <v>85</v>
+      </c>
+      <c r="I25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1257,22 +1551,28 @@
         <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26">
         <v>4010</v>
       </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>27</v>
+      <c r="F26">
+        <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H26" t="s">
+        <v>86</v>
+      </c>
+      <c r="I26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1280,45 +1580,54 @@
         <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27">
         <v>5000</v>
       </c>
-      <c r="E27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" t="s">
-        <v>28</v>
+      <c r="F27">
+        <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H27" t="s">
+        <v>87</v>
+      </c>
+      <c r="I27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
         <v>101</v>
       </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28">
+      <c r="D28" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28">
         <v>5051</v>
       </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" t="s">
-        <v>29</v>
+      <c r="F28">
+        <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1326,22 +1635,28 @@
         <v>105</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29">
         <v>5100</v>
       </c>
-      <c r="E29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" t="s">
-        <v>30</v>
+      <c r="F29">
+        <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H29" t="s">
+        <v>89</v>
+      </c>
+      <c r="I29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1349,22 +1664,28 @@
         <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30">
         <v>5130</v>
       </c>
-      <c r="E30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" t="s">
-        <v>31</v>
+      <c r="F30">
+        <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H30" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1372,22 +1693,28 @@
         <v>109</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31">
+        <v>25</v>
+      </c>
+      <c r="D31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31">
         <v>5200</v>
       </c>
-      <c r="E31" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" t="s">
-        <v>32</v>
+      <c r="F31">
+        <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1395,22 +1722,28 @@
         <v>111</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32">
         <v>5205</v>
       </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" t="s">
-        <v>33</v>
+      <c r="F32">
+        <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1418,22 +1751,28 @@
         <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33">
         <v>5220</v>
       </c>
-      <c r="E33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" t="s">
-        <v>34</v>
+      <c r="F33">
+        <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H33" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1441,22 +1780,28 @@
         <v>115</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34">
         <v>5250</v>
       </c>
-      <c r="E34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" t="s">
-        <v>35</v>
+      <c r="F34">
+        <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H34" t="s">
+        <v>94</v>
+      </c>
+      <c r="I34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1464,22 +1809,28 @@
         <v>117</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35">
+        <v>29</v>
+      </c>
+      <c r="D35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35">
         <v>5300</v>
       </c>
-      <c r="E35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" t="s">
-        <v>36</v>
+      <c r="F35">
+        <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H35" t="s">
+        <v>95</v>
+      </c>
+      <c r="I35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1487,22 +1838,28 @@
         <v>119</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36">
         <v>5500</v>
       </c>
-      <c r="E36" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" t="s">
-        <v>37</v>
+      <c r="F36">
+        <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H36" t="s">
+        <v>96</v>
+      </c>
+      <c r="I36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1510,22 +1867,28 @@
         <v>121</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37">
+        <v>31</v>
+      </c>
+      <c r="D37" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37">
         <v>5510</v>
       </c>
-      <c r="E37" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" t="s">
-        <v>38</v>
+      <c r="F37">
+        <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H37" t="s">
+        <v>97</v>
+      </c>
+      <c r="I37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1533,22 +1896,28 @@
         <v>123</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38">
+        <v>32</v>
+      </c>
+      <c r="D38" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38">
         <v>5535</v>
       </c>
-      <c r="E38" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" t="s">
-        <v>39</v>
+      <c r="F38">
+        <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H38" t="s">
+        <v>98</v>
+      </c>
+      <c r="I38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1556,22 +1925,28 @@
         <v>125</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39">
+        <v>33</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39">
         <v>5620</v>
       </c>
-      <c r="E39" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" t="s">
-        <v>40</v>
+      <c r="F39">
+        <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H39" t="s">
+        <v>99</v>
+      </c>
+      <c r="I39" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1579,22 +1954,28 @@
         <v>127</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40">
+        <v>34</v>
+      </c>
+      <c r="D40" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40">
         <v>5630</v>
       </c>
-      <c r="E40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" t="s">
-        <v>41</v>
+      <c r="F40">
+        <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H40" t="s">
+        <v>100</v>
+      </c>
+      <c r="I40" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1602,22 +1983,28 @@
         <v>129</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41">
+        <v>35</v>
+      </c>
+      <c r="D41" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41">
         <v>5650</v>
       </c>
-      <c r="E41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" t="s">
-        <v>42</v>
+      <c r="F41">
+        <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H41" t="s">
+        <v>101</v>
+      </c>
+      <c r="I41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1625,22 +2012,28 @@
         <v>131</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42">
+        <v>36</v>
+      </c>
+      <c r="D42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42">
         <v>5700</v>
       </c>
-      <c r="E42" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" t="s">
-        <v>43</v>
+      <c r="F42">
+        <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H42" t="s">
+        <v>102</v>
+      </c>
+      <c r="I42" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1648,22 +2041,28 @@
         <v>133</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43">
         <v>5800</v>
       </c>
-      <c r="E43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" t="s">
-        <v>44</v>
+      <c r="F43">
+        <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H43" t="s">
+        <v>103</v>
+      </c>
+      <c r="I43" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1671,22 +2070,28 @@
         <v>146</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44">
+        <v>38</v>
+      </c>
+      <c r="D44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44">
         <v>5960</v>
       </c>
-      <c r="E44" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" t="s">
-        <v>45</v>
+      <c r="F44">
+        <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H44" t="s">
+        <v>104</v>
+      </c>
+      <c r="I44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1694,22 +2099,28 @@
         <v>152</v>
       </c>
       <c r="C45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45">
+        <v>5960</v>
+      </c>
+      <c r="F45">
         <v>6</v>
       </c>
-      <c r="D45">
-        <v>5960</v>
-      </c>
-      <c r="E45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F45" t="s">
-        <v>46</v>
-      </c>
       <c r="G45" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H45" t="s">
+        <v>105</v>
+      </c>
+      <c r="I45" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1717,45 +2128,54 @@
         <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46">
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46">
         <v>6025</v>
       </c>
-      <c r="E46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" t="s">
-        <v>47</v>
+      <c r="F46">
+        <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H46" t="s">
+        <v>106</v>
+      </c>
+      <c r="I46" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47">
         <v>156</v>
       </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47">
+      <c r="D47" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47">
         <v>6051</v>
       </c>
-      <c r="E47" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" t="s">
-        <v>48</v>
+      <c r="F47">
+        <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H47" t="s">
+        <v>107</v>
+      </c>
+      <c r="I47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1763,22 +2183,28 @@
         <v>160</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48">
+        <v>41</v>
+      </c>
+      <c r="D48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48">
         <v>6100</v>
       </c>
-      <c r="E48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" t="s">
-        <v>30</v>
+      <c r="F48">
+        <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H48" t="s">
+        <v>89</v>
+      </c>
+      <c r="I48" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1786,22 +2212,28 @@
         <v>162</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49">
+        <v>42</v>
+      </c>
+      <c r="D49" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49">
         <v>6130</v>
       </c>
-      <c r="E49" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" t="s">
-        <v>31</v>
+      <c r="F49">
+        <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H49" t="s">
+        <v>90</v>
+      </c>
+      <c r="I49" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1809,22 +2241,28 @@
         <v>164</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50">
+        <v>43</v>
+      </c>
+      <c r="D50" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50">
         <v>6200</v>
       </c>
-      <c r="E50" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" t="s">
-        <v>32</v>
+      <c r="F50">
+        <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H50" t="s">
+        <v>91</v>
+      </c>
+      <c r="I50" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1832,22 +2270,28 @@
         <v>166</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51">
+        <v>44</v>
+      </c>
+      <c r="D51" t="s">
+        <v>65</v>
+      </c>
+      <c r="E51">
         <v>6205</v>
       </c>
-      <c r="E51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" t="s">
-        <v>33</v>
+      <c r="F51">
+        <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H51" t="s">
+        <v>92</v>
+      </c>
+      <c r="I51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1855,22 +2299,28 @@
         <v>168</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52">
+        <v>45</v>
+      </c>
+      <c r="D52" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52">
         <v>6220</v>
       </c>
-      <c r="E52" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" t="s">
-        <v>34</v>
+      <c r="F52">
+        <v>1</v>
       </c>
       <c r="G52" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H52" t="s">
+        <v>93</v>
+      </c>
+      <c r="I52" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1878,22 +2328,28 @@
         <v>170</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53">
+        <v>46</v>
+      </c>
+      <c r="D53" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53">
         <v>6225</v>
       </c>
-      <c r="E53" t="s">
-        <v>7</v>
-      </c>
-      <c r="F53" t="s">
-        <v>49</v>
+      <c r="F53">
+        <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H53" t="s">
+        <v>108</v>
+      </c>
+      <c r="I53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1901,22 +2357,28 @@
         <v>172</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54">
+        <v>47</v>
+      </c>
+      <c r="D54" t="s">
+        <v>65</v>
+      </c>
+      <c r="E54">
         <v>6250</v>
       </c>
-      <c r="E54" t="s">
-        <v>7</v>
-      </c>
-      <c r="F54" t="s">
-        <v>35</v>
+      <c r="F54">
+        <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H54" t="s">
+        <v>94</v>
+      </c>
+      <c r="I54" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1924,22 +2386,28 @@
         <v>174</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55">
+        <v>48</v>
+      </c>
+      <c r="D55" t="s">
+        <v>65</v>
+      </c>
+      <c r="E55">
         <v>6300</v>
       </c>
-      <c r="E55" t="s">
-        <v>7</v>
-      </c>
-      <c r="F55" t="s">
-        <v>50</v>
+      <c r="F55">
+        <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H55" t="s">
+        <v>109</v>
+      </c>
+      <c r="I55" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1947,22 +2415,28 @@
         <v>176</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56">
+        <v>49</v>
+      </c>
+      <c r="D56" t="s">
+        <v>65</v>
+      </c>
+      <c r="E56">
         <v>6500</v>
       </c>
-      <c r="E56" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" t="s">
-        <v>37</v>
+      <c r="F56">
+        <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H56" t="s">
+        <v>96</v>
+      </c>
+      <c r="I56" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1970,22 +2444,28 @@
         <v>178</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57">
+        <v>50</v>
+      </c>
+      <c r="D57" t="s">
+        <v>65</v>
+      </c>
+      <c r="E57">
         <v>6510</v>
       </c>
-      <c r="E57" t="s">
-        <v>7</v>
-      </c>
-      <c r="F57" t="s">
-        <v>38</v>
+      <c r="F57">
+        <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H57" t="s">
+        <v>97</v>
+      </c>
+      <c r="I57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1993,22 +2473,28 @@
         <v>180</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58">
+        <v>51</v>
+      </c>
+      <c r="D58" t="s">
+        <v>65</v>
+      </c>
+      <c r="E58">
         <v>6535</v>
       </c>
-      <c r="E58" t="s">
-        <v>7</v>
-      </c>
-      <c r="F58" t="s">
-        <v>39</v>
+      <c r="F58">
+        <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H58" t="s">
+        <v>98</v>
+      </c>
+      <c r="I58" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2016,22 +2502,28 @@
         <v>182</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59">
+        <v>52</v>
+      </c>
+      <c r="D59" t="s">
+        <v>65</v>
+      </c>
+      <c r="E59">
         <v>6620</v>
       </c>
-      <c r="E59" t="s">
-        <v>7</v>
-      </c>
-      <c r="F59" t="s">
-        <v>40</v>
+      <c r="F59">
+        <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H59" t="s">
+        <v>99</v>
+      </c>
+      <c r="I59" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2039,22 +2531,28 @@
         <v>184</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60">
+        <v>53</v>
+      </c>
+      <c r="D60" t="s">
+        <v>65</v>
+      </c>
+      <c r="E60">
         <v>6630</v>
       </c>
-      <c r="E60" t="s">
-        <v>7</v>
-      </c>
-      <c r="F60" t="s">
-        <v>41</v>
+      <c r="F60">
+        <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H60" t="s">
+        <v>100</v>
+      </c>
+      <c r="I60" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2062,22 +2560,28 @@
         <v>186</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61">
+        <v>54</v>
+      </c>
+      <c r="D61" t="s">
+        <v>65</v>
+      </c>
+      <c r="E61">
         <v>6650</v>
       </c>
-      <c r="E61" t="s">
-        <v>7</v>
-      </c>
-      <c r="F61" t="s">
-        <v>42</v>
+      <c r="F61">
+        <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H61" t="s">
+        <v>101</v>
+      </c>
+      <c r="I61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2085,22 +2589,28 @@
         <v>188</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62">
+        <v>55</v>
+      </c>
+      <c r="D62" t="s">
+        <v>65</v>
+      </c>
+      <c r="E62">
         <v>6700</v>
       </c>
-      <c r="E62" t="s">
-        <v>7</v>
-      </c>
-      <c r="F62" t="s">
-        <v>43</v>
+      <c r="F62">
+        <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H62" t="s">
+        <v>102</v>
+      </c>
+      <c r="I62" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2108,22 +2618,28 @@
         <v>190</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63">
+        <v>56</v>
+      </c>
+      <c r="D63" t="s">
+        <v>65</v>
+      </c>
+      <c r="E63">
         <v>6800</v>
       </c>
-      <c r="E63" t="s">
-        <v>7</v>
-      </c>
-      <c r="F63" t="s">
-        <v>44</v>
+      <c r="F63">
+        <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H63" t="s">
+        <v>103</v>
+      </c>
+      <c r="I63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2131,22 +2647,28 @@
         <v>198</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64">
+        <v>57</v>
+      </c>
+      <c r="D64" t="s">
+        <v>65</v>
+      </c>
+      <c r="E64">
         <v>6960</v>
       </c>
-      <c r="E64" t="s">
-        <v>7</v>
-      </c>
-      <c r="F64" t="s">
-        <v>45</v>
+      <c r="F64">
+        <v>2</v>
       </c>
       <c r="G64" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H64" t="s">
+        <v>104</v>
+      </c>
+      <c r="I64" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2154,22 +2676,28 @@
         <v>204</v>
       </c>
       <c r="C65" t="s">
+        <v>58</v>
+      </c>
+      <c r="D65" t="s">
+        <v>65</v>
+      </c>
+      <c r="E65">
+        <v>6960</v>
+      </c>
+      <c r="F65">
         <v>6</v>
       </c>
-      <c r="D65">
-        <v>6960</v>
-      </c>
-      <c r="E65" t="s">
-        <v>7</v>
-      </c>
-      <c r="F65" t="s">
-        <v>46</v>
-      </c>
       <c r="G65" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H65" t="s">
+        <v>105</v>
+      </c>
+      <c r="I65" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2177,22 +2705,28 @@
         <v>206</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66">
+        <v>59</v>
+      </c>
+      <c r="D66" t="s">
+        <v>65</v>
+      </c>
+      <c r="E66">
         <v>6960</v>
       </c>
-      <c r="E66" t="s">
-        <v>7</v>
-      </c>
-      <c r="F66" t="s">
-        <v>21</v>
+      <c r="F66">
+        <v>9</v>
       </c>
       <c r="G66" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H66" t="s">
+        <v>80</v>
+      </c>
+      <c r="I66" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2200,22 +2734,28 @@
         <v>212</v>
       </c>
       <c r="C67" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67">
+        <v>60</v>
+      </c>
+      <c r="D67" t="s">
+        <v>65</v>
+      </c>
+      <c r="E67">
         <v>7230</v>
       </c>
-      <c r="E67" t="s">
-        <v>7</v>
-      </c>
-      <c r="F67" t="s">
-        <v>51</v>
+      <c r="F67">
+        <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H67" t="s">
+        <v>110</v>
+      </c>
+      <c r="I67" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2223,22 +2763,28 @@
         <v>213</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68">
+        <v>61</v>
+      </c>
+      <c r="D68" t="s">
+        <v>65</v>
+      </c>
+      <c r="E68">
         <v>7660</v>
       </c>
-      <c r="E68" t="s">
-        <v>7</v>
-      </c>
-      <c r="F68" t="s">
-        <v>52</v>
+      <c r="F68">
+        <v>1</v>
       </c>
       <c r="G68" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="H68" t="s">
+        <v>111</v>
+      </c>
+      <c r="I68" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2246,22 +2792,28 @@
         <v>214</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69">
+        <v>62</v>
+      </c>
+      <c r="D69" t="s">
+        <v>65</v>
+      </c>
+      <c r="E69">
         <v>7960</v>
       </c>
-      <c r="E69" t="s">
-        <v>8</v>
-      </c>
-      <c r="F69" t="s">
-        <v>53</v>
+      <c r="F69">
+        <v>1</v>
       </c>
       <c r="G69" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
+        <v>67</v>
+      </c>
+      <c r="H69" t="s">
+        <v>112</v>
+      </c>
+      <c r="I69" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2269,22 +2821,28 @@
         <v>216</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70">
+        <v>63</v>
+      </c>
+      <c r="D70" t="s">
+        <v>65</v>
+      </c>
+      <c r="E70">
         <v>7960</v>
       </c>
-      <c r="E70" t="s">
-        <v>8</v>
-      </c>
-      <c r="F70" t="s">
-        <v>54</v>
+      <c r="F70">
+        <v>2</v>
       </c>
       <c r="G70" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
+        <v>67</v>
+      </c>
+      <c r="H70" t="s">
+        <v>113</v>
+      </c>
+      <c r="I70" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2292,19 +2850,25 @@
         <v>217</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71">
+        <v>64</v>
+      </c>
+      <c r="D71" t="s">
+        <v>65</v>
+      </c>
+      <c r="E71">
         <v>7960</v>
       </c>
-      <c r="E71" t="s">
-        <v>8</v>
-      </c>
-      <c r="F71" t="s">
-        <v>55</v>
+      <c r="F71">
+        <v>4</v>
       </c>
       <c r="G71" t="s">
-        <v>99</v>
+        <v>67</v>
+      </c>
+      <c r="H71" t="s">
+        <v>114</v>
+      </c>
+      <c r="I71" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>